<commit_message>
CE06ISSM changed reference designators to match 1100-00006 ver 1-27
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE06ISSM_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CE06ISSM_00003.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="766" activeTab="1"/>
   </bookViews>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="214">
   <si>
     <t>Ref Des</t>
   </si>
@@ -672,6 +677,12 @@
   </si>
   <si>
     <t>CE06ISSM-SBD17-06-FLORTD000</t>
+  </si>
+  <si>
+    <t>A01755</t>
+  </si>
+  <si>
+    <t>A00219</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1655,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1679,7 +1690,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2009,9 +2020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,744 +3100,950 @@
       <c r="AML2"/>
     </row>
     <row r="3" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J3" s="24" t="s">
+      <c r="A3" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="22">
+      <c r="D3" s="22">
         <v>3</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="E3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="G3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="44">
+      <c r="H3" s="44">
         <v>47.133266999999996</v>
       </c>
-      <c r="P3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J4" s="24" t="s">
+      <c r="A4" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L4" s="22">
+      <c r="D4" s="22">
         <v>3</v>
       </c>
-      <c r="M4" s="43" t="s">
+      <c r="E4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="G4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="44">
+      <c r="H4" s="44">
         <v>-124.270917</v>
       </c>
-      <c r="P4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J5" s="24" t="s">
+      <c r="A5" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L5" s="22">
+      <c r="D5" s="22">
         <v>3</v>
       </c>
-      <c r="M5" s="43" t="s">
+      <c r="E5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F5" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="G5" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="45">
+      <c r="H5" s="45">
         <v>1.21059323E-3</v>
       </c>
-      <c r="P5" s="26"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J6" s="24" t="s">
+      <c r="A6" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L6" s="22">
+      <c r="D6" s="22">
         <v>3</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="E6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="G6" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="O6" s="45">
+      <c r="H6" s="45">
         <v>2.8481035700000002E-4</v>
       </c>
-      <c r="P6" s="27"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J7" s="24" t="s">
+      <c r="A7" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L7" s="22">
+      <c r="D7" s="22">
         <v>3</v>
       </c>
-      <c r="M7" s="43" t="s">
+      <c r="E7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="G7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="45">
+      <c r="H7" s="45">
         <v>-2.1758474099999998E-6</v>
       </c>
-      <c r="P7" s="26"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J8" s="24" t="s">
+      <c r="A8" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L8" s="22">
+      <c r="D8" s="22">
         <v>3</v>
       </c>
-      <c r="M8" s="43" t="s">
+      <c r="E8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F8" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="G8" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O8" s="45">
+      <c r="H8" s="45">
         <v>2.29626898E-7</v>
       </c>
-      <c r="P8" s="28"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J9" s="24" t="s">
+      <c r="A9" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="22">
+      <c r="D9" s="22">
         <v>3</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="E9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="G9" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="O9" s="45">
+      <c r="H9" s="45">
         <v>101.261408</v>
       </c>
-      <c r="P9"/>
+      <c r="I9"/>
     </row>
     <row r="10" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J10" s="24" t="s">
+      <c r="A10" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L10" s="22">
+      <c r="D10" s="22">
         <v>3</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="E10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F10" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N10" s="22" t="s">
+      <c r="G10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="O10" s="45">
+      <c r="H10" s="45">
         <v>-41.7521238</v>
       </c>
-      <c r="P10"/>
+      <c r="I10"/>
     </row>
     <row r="11" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J11" s="24" t="s">
+      <c r="A11" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="B11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L11" s="22">
+      <c r="D11" s="22">
         <v>3</v>
       </c>
-      <c r="M11" s="43" t="s">
+      <c r="E11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F11" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="G11" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="O11" s="45">
+      <c r="H11" s="45">
         <v>-1.19072143</v>
       </c>
-      <c r="P11"/>
+      <c r="I11"/>
     </row>
     <row r="12" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J12" s="24" t="s">
+      <c r="A12" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="B12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L12" s="22">
+      <c r="D12" s="22">
         <v>3</v>
       </c>
-      <c r="M12" s="43" t="s">
+      <c r="E12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F12" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N12" s="22" t="s">
+      <c r="G12" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="O12" s="45">
+      <c r="H12" s="45">
         <v>518916.52299999999</v>
       </c>
-      <c r="P12"/>
+      <c r="I12"/>
     </row>
     <row r="13" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J13" s="24" t="s">
+      <c r="A13" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L13" s="22">
+      <c r="D13" s="22">
         <v>3</v>
       </c>
-      <c r="M13" s="43" t="s">
+      <c r="E13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F13" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="G13" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="O13" s="45">
+      <c r="H13" s="45">
         <v>-156.07004599999999</v>
       </c>
-      <c r="P13"/>
+      <c r="I13"/>
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J14" s="24" t="s">
+      <c r="A14" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="B14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L14" s="22">
+      <c r="D14" s="22">
         <v>3</v>
       </c>
-      <c r="M14" s="43" t="s">
+      <c r="E14" t="s">
+        <v>212</v>
+      </c>
+      <c r="F14" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N14" s="22" t="s">
+      <c r="G14" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="O14" s="45">
+      <c r="H14" s="45">
         <v>-1.4203462899999999</v>
       </c>
-      <c r="P14"/>
+      <c r="I14"/>
     </row>
     <row r="15" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J15" s="24" t="s">
+      <c r="A15" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="B15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L15" s="22">
+      <c r="D15" s="22">
         <v>3</v>
       </c>
-      <c r="M15" s="43" t="s">
+      <c r="E15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N15" s="22" t="s">
+      <c r="G15" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="O15" s="45">
+      <c r="H15" s="45">
         <v>25.026875</v>
       </c>
-      <c r="P15"/>
+      <c r="I15"/>
     </row>
     <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J16" s="24" t="s">
+      <c r="A16" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="B16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L16" s="22">
+      <c r="D16" s="22">
         <v>3</v>
       </c>
-      <c r="M16" s="43" t="s">
+      <c r="E16" t="s">
+        <v>212</v>
+      </c>
+      <c r="F16" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="G16" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="O16" s="45">
+      <c r="H16" s="45">
         <v>7.7499999999999997E-4</v>
       </c>
-      <c r="P16"/>
+      <c r="I16"/>
     </row>
-    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J17" s="24" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="B17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L17" s="22">
+      <c r="D17" s="22">
         <v>3</v>
       </c>
-      <c r="M17" s="43" t="s">
+      <c r="E17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N17" s="22" t="s">
+      <c r="G17" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="O17" s="45">
+      <c r="H17" s="45">
         <v>0</v>
       </c>
-      <c r="P17"/>
+      <c r="I17"/>
     </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J18" s="24" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="B18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L18" s="22">
+      <c r="D18" s="22">
         <v>3</v>
       </c>
-      <c r="M18" s="43" t="s">
+      <c r="E18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N18" s="22" t="s">
+      <c r="G18" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="O18" s="45">
+      <c r="H18" s="45">
         <v>-2.6785821699999999</v>
       </c>
-      <c r="P18"/>
+      <c r="I18"/>
     </row>
-    <row r="19" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J19" s="24" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="B19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L19" s="22">
+      <c r="D19" s="22">
         <v>3</v>
       </c>
-      <c r="M19" s="43" t="s">
+      <c r="E19" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N19" s="22" t="s">
+      <c r="G19" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="O19" s="45">
+      <c r="H19" s="45">
         <v>6.2104943900000002E-4</v>
       </c>
-      <c r="P19"/>
+      <c r="I19"/>
     </row>
-    <row r="20" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J20" s="24" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K20" s="22" t="s">
+      <c r="B20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L20" s="22">
+      <c r="D20" s="22">
         <v>3</v>
       </c>
-      <c r="M20" s="43" t="s">
+      <c r="E20" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N20" s="22" t="s">
+      <c r="G20" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="O20" s="45">
+      <c r="H20" s="45">
         <v>8.9875144600000006E-12</v>
       </c>
-      <c r="P20"/>
+      <c r="I20"/>
     </row>
-    <row r="21" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J21" s="24" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="B21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L21" s="22">
+      <c r="D21" s="22">
         <v>3</v>
       </c>
-      <c r="M21" s="43" t="s">
+      <c r="E21" t="s">
+        <v>212</v>
+      </c>
+      <c r="F21" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N21" s="22" t="s">
+      <c r="G21" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="O21" s="45">
+      <c r="H21" s="45">
         <v>-0.97856695599999999</v>
       </c>
-      <c r="P21"/>
+      <c r="I21"/>
     </row>
-    <row r="22" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J22" s="24" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K22" s="22" t="s">
+      <c r="B22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L22" s="22">
+      <c r="D22" s="22">
         <v>3</v>
       </c>
-      <c r="M22" s="43" t="s">
+      <c r="E22" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N22" s="22" t="s">
+      <c r="G22" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="O22" s="45">
+      <c r="H22" s="45">
         <v>0.15168742700000001</v>
       </c>
-      <c r="P22"/>
+      <c r="I22"/>
     </row>
-    <row r="23" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J23" s="24" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K23" s="22" t="s">
+      <c r="B23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L23" s="22">
+      <c r="D23" s="22">
         <v>3</v>
       </c>
-      <c r="M23" s="43" t="s">
+      <c r="E23" t="s">
+        <v>212</v>
+      </c>
+      <c r="F23" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N23" s="22" t="s">
+      <c r="G23" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="O23" s="45">
+      <c r="H23" s="45">
         <v>-1.15940192E-4</v>
       </c>
-      <c r="P23"/>
+      <c r="I23"/>
     </row>
-    <row r="24" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J24" s="24" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K24" s="22" t="s">
+      <c r="B24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L24" s="22">
+      <c r="D24" s="22">
         <v>3</v>
       </c>
-      <c r="M24" s="43" t="s">
+      <c r="E24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F24" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N24" s="22" t="s">
+      <c r="G24" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="O24" s="45">
+      <c r="H24" s="45">
         <v>3.1292238999999998E-5</v>
       </c>
-      <c r="P24"/>
+      <c r="I24"/>
     </row>
-    <row r="25" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J25" s="24" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K25" s="22" t="s">
+      <c r="B25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L25" s="22">
+      <c r="D25" s="22">
         <v>3</v>
       </c>
-      <c r="M25" s="43" t="s">
+      <c r="E25" t="s">
+        <v>212</v>
+      </c>
+      <c r="F25" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N25" s="22" t="s">
+      <c r="G25" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="O25" s="45">
+      <c r="H25" s="45">
         <v>-9.5700000000000003E-8</v>
       </c>
-      <c r="P25"/>
+      <c r="I25"/>
     </row>
-    <row r="26" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J26" s="24" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K26" s="22" t="s">
+      <c r="B26" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L26" s="22">
+      <c r="D26" s="22">
         <v>3</v>
       </c>
-      <c r="M26" s="43" t="s">
+      <c r="E26" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="N26" s="22" t="s">
+      <c r="G26" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="O26" s="45">
+      <c r="H26" s="45">
         <v>3.2499999999999998E-6</v>
       </c>
-      <c r="P26"/>
+      <c r="I26"/>
     </row>
-    <row r="27" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-      <c r="O27" s="23"/>
-      <c r="P27"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="F27"/>
+      <c r="H27" s="23"/>
+      <c r="I27"/>
     </row>
-    <row r="28" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J28" s="22" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="B28" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L28" s="22">
+      <c r="D28" s="22">
         <v>3</v>
       </c>
-      <c r="M28" s="43">
+      <c r="E28" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="43">
         <v>996</v>
       </c>
-      <c r="N28" s="22" t="s">
+      <c r="G28" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O28" s="46">
+      <c r="H28" s="46">
         <v>47</v>
       </c>
-      <c r="P28"/>
+      <c r="I28"/>
     </row>
-    <row r="29" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J29" s="22" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="B29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L29" s="22">
+      <c r="D29" s="22">
         <v>3</v>
       </c>
-      <c r="M29" s="43">
+      <c r="E29" t="s">
+        <v>213</v>
+      </c>
+      <c r="F29" s="43">
         <v>996</v>
       </c>
-      <c r="N29" s="22" t="s">
+      <c r="G29" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="O29" s="46">
+      <c r="H29" s="46">
         <v>1.734E-6</v>
       </c>
-      <c r="P29"/>
+      <c r="I29"/>
     </row>
-    <row r="30" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J30" s="22" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="B30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L30" s="22">
+      <c r="D30" s="22">
         <v>3</v>
       </c>
-      <c r="M30" s="43">
+      <c r="E30" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" s="43">
         <v>996</v>
       </c>
-      <c r="N30" s="22" t="s">
+      <c r="G30" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="O30" s="46">
+      <c r="H30" s="46">
         <v>49</v>
       </c>
-      <c r="P30"/>
+      <c r="I30"/>
     </row>
-    <row r="31" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J31" s="22" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="B31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L31" s="22">
+      <c r="D31" s="22">
         <v>3</v>
       </c>
-      <c r="M31" s="43">
+      <c r="E31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="43">
         <v>996</v>
       </c>
-      <c r="N31" s="22" t="s">
+      <c r="G31" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="O31" s="46">
+      <c r="H31" s="46">
         <v>1.17E-2</v>
       </c>
-      <c r="P31"/>
+      <c r="I31"/>
     </row>
-    <row r="32" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J32" s="22" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K32" s="22" t="s">
+      <c r="B32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L32" s="22">
+      <c r="D32" s="22">
         <v>3</v>
       </c>
-      <c r="M32" s="43">
+      <c r="E32" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" s="43">
         <v>996</v>
       </c>
-      <c r="N32" s="22" t="s">
+      <c r="G32" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O32" s="46">
+      <c r="H32" s="46">
         <v>44</v>
       </c>
-      <c r="P32"/>
+      <c r="I32"/>
     </row>
     <row r="33" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J33" s="22" t="s">
+      <c r="A33" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K33" s="22" t="s">
+      <c r="B33" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L33" s="22">
+      <c r="D33" s="22">
         <v>3</v>
       </c>
-      <c r="M33" s="43">
+      <c r="E33" t="s">
+        <v>213</v>
+      </c>
+      <c r="F33" s="43">
         <v>996</v>
       </c>
-      <c r="N33" s="22" t="s">
+      <c r="G33" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O33" s="46">
+      <c r="H33" s="46">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="P33"/>
+      <c r="I33"/>
     </row>
     <row r="34" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J34" s="22" t="s">
+      <c r="A34" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K34" s="22" t="s">
+      <c r="B34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L34" s="22">
+      <c r="D34" s="22">
         <v>3</v>
       </c>
-      <c r="M34" s="43">
+      <c r="E34" t="s">
+        <v>213</v>
+      </c>
+      <c r="F34" s="43">
         <v>996</v>
       </c>
-      <c r="N34" s="22" t="s">
+      <c r="G34" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="O34" s="46">
+      <c r="H34" s="46">
         <v>124</v>
       </c>
-      <c r="P34" s="22" t="s">
+      <c r="I34" s="22" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J35" s="22" t="s">
+      <c r="A35" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K35" s="22" t="s">
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L35" s="22">
+      <c r="D35" s="22">
         <v>3</v>
       </c>
-      <c r="M35" s="43">
+      <c r="E35" t="s">
+        <v>213</v>
+      </c>
+      <c r="F35" s="43">
         <v>996</v>
       </c>
-      <c r="N35" s="22" t="s">
+      <c r="G35" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="O35" s="46">
+      <c r="H35" s="46">
         <v>700</v>
       </c>
-      <c r="P35" s="22" t="s">
+      <c r="I35" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J36" s="22" t="s">
+      <c r="A36" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K36" s="22" t="s">
+      <c r="B36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L36" s="22">
+      <c r="D36" s="22">
         <v>3</v>
       </c>
-      <c r="M36" s="43">
+      <c r="E36" t="s">
+        <v>213</v>
+      </c>
+      <c r="F36" s="43">
         <v>996</v>
       </c>
-      <c r="N36" s="22" t="s">
+      <c r="G36" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="O36" s="46">
+      <c r="H36" s="46">
         <v>1.0760000000000001</v>
       </c>
-      <c r="P36" s="22" t="s">
+      <c r="I36" s="22" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="J37" s="22" t="s">
+      <c r="A37" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="K37" s="22" t="s">
+      <c r="B37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="L37" s="22">
+      <c r="D37" s="22">
         <v>3</v>
       </c>
-      <c r="M37" s="43">
+      <c r="E37" t="s">
+        <v>213</v>
+      </c>
+      <c r="F37" s="43">
         <v>996</v>
       </c>
-      <c r="N37" s="22" t="s">
+      <c r="G37" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="O37" s="46">
+      <c r="H37" s="46">
         <v>3.9E-2</v>
       </c>
-      <c r="P37" s="22" t="s">
+      <c r="I37" s="22" t="s">
         <v>29</v>
       </c>
+      <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A38"/>
-      <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
       <c r="F38"/>
-      <c r="H38" s="23"/>
-      <c r="I38"/>
+      <c r="G38"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23"/>
+      <c r="J38"/>
     </row>
     <row r="39" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">

</xml_diff>